<commit_message>
Update Notification Center: default to tomorrow, add send button, and refresh excel report
</commit_message>
<xml_diff>
--- a/reporte_agendas.xlsx
+++ b/reporte_agendas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>PENDIENTE</t>
+          <t>COMPLETADO</t>
         </is>
       </c>
     </row>
@@ -4804,6 +4804,306 @@
       <c r="L73" t="inlineStr">
         <is>
           <t>COMPLETADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>18:00:00</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>53166674</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>AGUIRRE, GUILLERMINA</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>3794630005</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>IOSCOR</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v>12</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>EEG</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>ELECTRO Y MAPEOS</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>DR. MONZON ROMILIO</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>COMPLETADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>18:00:00</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>30141716</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>AGUIRRE, ALFREDO RAUL</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>3794630005</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>OSDE</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>42</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>TAC COMPLETA DE ABDOMEN</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>TOMOGRAFIAS Y RX</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>DR. MONZON ROMILIO</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>COMPLETADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>19:00:00</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>30141716</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>AGUIRRE, ALFREDO RAUL</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>3794630005</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>OSDE</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>42</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>TAC DE CEREBRO</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>TOMOGRAFIAS Y RX</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>RAINERO FEDERICO</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>COMPLETADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>19:00:00</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>30141716</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>AGUIRRE, ALFREDO RAUL</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>3794630005</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>OSDE</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="H77" t="n">
+        <v>42</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>TAC DE CUELLO</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>TOMOGRAFIAS Y RX</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>RAINERO FEDERICO</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>COMPLETADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>22/12/2025</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>31648199</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>VALLEJOS SCHULZE, MARIA ELENA</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>3794774785</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>IOSCOR</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>40</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>CENTELLOGRAMA DE TIROIDES</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>CAMARA GAMMA</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>DE LOS REYES</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>PENDIENTE</t>
         </is>
       </c>
     </row>

</xml_diff>